<commit_message>
#test case and flow chart
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ceburns1\PycharmProjects\cs151-sky-caitlin_leif_lab3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B39C795-C7D1-5241-9421-DFCBA04D9A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5565579D-70FE-4F36-AE9E-14924A2D13D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="67920" windowHeight="28300" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="7095" yWindow="300" windowWidth="21600" windowHeight="11295" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Test Description</t>
   </si>
@@ -187,15 +187,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -208,11 +199,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -232,9 +232,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -272,7 +272,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -378,7 +378,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -520,7 +520,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -531,231 +531,322 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="1">
         <v>46</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="1">
         <v>2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="1">
         <v>90</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="6"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="1">
         <v>70</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="1">
         <v>1.8</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="1">
         <v>120</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="6"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
       <c r="D7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="s">
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" ht="46" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="J7" s="9"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" ht="31" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" ht="31" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
+      <c r="B9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10</v>
+      </c>
+      <c r="D9" s="1">
+        <f>IF(B9=$A$3,B$3,B$4)</f>
+        <v>46</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2</v>
+      </c>
+      <c r="F9" s="1">
+        <v>90</v>
+      </c>
+      <c r="G9" s="1">
+        <f>SQRT((2*D9)/9.8)</f>
+        <v>3.0639443699324591</v>
+      </c>
+      <c r="H9" s="2">
+        <f>C9*G9</f>
+        <v>30.639443699324591</v>
+      </c>
+      <c r="I9">
+        <f>C9*G9</f>
+        <v>30.639443699324591</v>
+      </c>
+      <c r="J9" s="2">
+        <f>60+(H9-F9)*E9</f>
+        <v>-58.721112601350825</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" ht="31" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1">
+        <f>IF(B9=$A$3,B$3,B$4)</f>
+        <v>46</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1">
+        <v>90</v>
+      </c>
+      <c r="G10" s="1">
+        <f>SQRT((2*D10)/9.8)</f>
+        <v>3.0639443699324591</v>
+      </c>
+      <c r="H10" s="2">
+        <f>C10*G10</f>
+        <v>76.598609248311476</v>
+      </c>
+      <c r="I10" s="2">
+        <f>C10*G10</f>
+        <v>76.598609248311476</v>
+      </c>
+      <c r="J10" s="2">
+        <f>60+(H10-F10)*E10</f>
+        <v>33.197218496622952</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" ht="31" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1">
+        <v>11</v>
+      </c>
+      <c r="D11" s="1">
+        <v>70</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="F11" s="1">
+        <v>120</v>
+      </c>
+      <c r="G11" s="1">
+        <f>SQRT((2*D11)/9.8)</f>
+        <v>3.7796447300922722</v>
+      </c>
+      <c r="H11" s="2">
+        <f>C11*G11</f>
+        <v>41.576092031014994</v>
+      </c>
+      <c r="I11" s="2">
+        <f>C11*G11</f>
+        <v>41.576092031014994</v>
+      </c>
+      <c r="J11" s="2">
+        <f>60+(H11-F11)*E11</f>
+        <v>-81.163034344173013</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1">
+        <v>28</v>
+      </c>
+      <c r="D12" s="1">
+        <v>70</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="F12" s="1">
+        <v>120</v>
+      </c>
+      <c r="G12" s="1">
+        <f>SQRT((2*D12)/9.8)</f>
+        <v>3.7796447300922722</v>
+      </c>
+      <c r="H12" s="2">
+        <f>C12*G12</f>
+        <v>105.83005244258362</v>
+      </c>
+      <c r="I12" s="2">
+        <f>C12*G12</f>
+        <v>105.83005244258362</v>
+      </c>
+      <c r="J12" s="2">
+        <f>60+(H12-F12)*E12</f>
+        <v>34.494094396650517</v>
+      </c>
+      <c r="K12" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>